<commit_message>
updated to use sqlalchemy
</commit_message>
<xml_diff>
--- a/data/data_dictionary.xlsx
+++ b/data/data_dictionary.xlsx
@@ -3371,10 +3371,14 @@
       </c>
       <c r="G25" t="inlineStr">
         <is>
-          <t>optional</t>
-        </is>
-      </c>
-      <c r="H25" t="inlineStr"/>
+          <t>minimal</t>
+        </is>
+      </c>
+      <c r="H25" t="inlineStr">
+        <is>
+          <t>([histopat] = '0')</t>
+        </is>
+      </c>
       <c r="I25" t="inlineStr">
         <is>
           <t>Yes ([histopat] = '0')</t>
@@ -3449,10 +3453,14 @@
       </c>
       <c r="G26" t="inlineStr">
         <is>
-          <t>optional</t>
-        </is>
-      </c>
-      <c r="H26" t="inlineStr"/>
+          <t>minimal</t>
+        </is>
+      </c>
+      <c r="H26" t="inlineStr">
+        <is>
+          <t>([histopat] = '0')</t>
+        </is>
+      </c>
       <c r="I26" t="inlineStr">
         <is>
           <t>Yes ([histopat] = '0')</t>
@@ -3527,10 +3535,14 @@
       </c>
       <c r="G27" t="inlineStr">
         <is>
-          <t>optional</t>
-        </is>
-      </c>
-      <c r="H27" t="inlineStr"/>
+          <t>minimal</t>
+        </is>
+      </c>
+      <c r="H27" t="inlineStr">
+        <is>
+          <t>([histopat] = '0')</t>
+        </is>
+      </c>
       <c r="I27" t="inlineStr">
         <is>
           <t>Yes ([histopat] = '0')</t>
@@ -3605,10 +3617,14 @@
       </c>
       <c r="G28" t="inlineStr">
         <is>
-          <t>optional</t>
-        </is>
-      </c>
-      <c r="H28" t="inlineStr"/>
+          <t>minimal</t>
+        </is>
+      </c>
+      <c r="H28" t="inlineStr">
+        <is>
+          <t>([histopat] = '0' AND [tnm_pt] = '')</t>
+        </is>
+      </c>
       <c r="I28" t="inlineStr">
         <is>
           <t>Yes ([histopat] = '0' AND [tnm_pt] = '')</t>
@@ -3683,10 +3699,14 @@
       </c>
       <c r="G29" t="inlineStr">
         <is>
-          <t>optional</t>
-        </is>
-      </c>
-      <c r="H29" t="inlineStr"/>
+          <t>minimal</t>
+        </is>
+      </c>
+      <c r="H29" t="inlineStr">
+        <is>
+          <t>([histopat] = '0' AND [tnm_pn] = '')</t>
+        </is>
+      </c>
       <c r="I29" t="inlineStr">
         <is>
           <t>Yes ([histopat] = '0' AND [tnm_pn] = '')</t>
@@ -3761,10 +3781,14 @@
       </c>
       <c r="G30" t="inlineStr">
         <is>
-          <t>optional</t>
-        </is>
-      </c>
-      <c r="H30" t="inlineStr"/>
+          <t>minimal</t>
+        </is>
+      </c>
+      <c r="H30" t="inlineStr">
+        <is>
+          <t>([histopat] = '0' AND [tnm_pm] = '')</t>
+        </is>
+      </c>
       <c r="I30" t="inlineStr">
         <is>
           <t>Yes ([histopat] = '0' AND [tnm_pm] = '')</t>
@@ -9080,17 +9104,17 @@
       </c>
       <c r="H31" t="inlineStr">
         <is>
-          <t>([her2ihq] = '2')</t>
+          <t>([her2ihc] = '2')</t>
         </is>
       </c>
       <c r="I31" t="inlineStr">
         <is>
-          <t>Yes ([her2ihq] = '2')</t>
+          <t>Yes ([her2ihc] = '2')</t>
         </is>
       </c>
       <c r="J31" t="inlineStr">
         <is>
-          <t>Yes ([her2ihq] = '2')</t>
+          <t>Yes ([her2ihc] = '2')</t>
         </is>
       </c>
       <c r="K31" t="inlineStr">
@@ -17450,9 +17474,9 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{27EDDEEA-1BDE-4439-BEE9-655B5C2DAF05}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1D467FC5-99AB-4DFD-B4C5-0732638C1026}"/>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F5B39A3D-09D5-4D1F-B707-D30F418CC073}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{4A3D23C0-AE02-4085-AC08-87E07DFDE0EE}"/>
 </file>
</xml_diff>